<commit_message>
Changed the contents button for sections to be "go to" instead of "edit", added in display.title functionality to contents and imnci survey
</commit_message>
<xml_diff>
--- a/form-files/tables/imnci/forms/imnci_test/imnci_test.xlsx
+++ b/form-files/tables/imnci/forms/imnci_test/imnci_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="540" windowWidth="47460" windowHeight="24020" firstSheet="1" activeTab="14"/>
+    <workbookView xWindow="1200" yWindow="460" windowWidth="47460" windowHeight="24020"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="10" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2824" uniqueCount="1331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2828" uniqueCount="1333">
   <si>
     <t>comments</t>
   </si>
@@ -4201,6 +4201,12 @@
   </si>
   <si>
     <t xml:space="preserve">hideInContents </t>
+  </si>
+  <si>
+    <t>Which symptoms does the child have?</t>
+  </si>
+  <si>
+    <t>Acknowledge that protocol does not support assessing a child under 2 months old.</t>
   </si>
 </sst>
 </file>
@@ -4562,10 +4568,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="34" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4756,12 +4764,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -5062,10 +5072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -5074,15 +5084,15 @@
     <col min="2" max="2" width="29.83203125" customWidth="1"/>
     <col min="3" max="3" width="32.83203125" customWidth="1"/>
     <col min="4" max="5" width="28.33203125" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="7" max="7" width="41.83203125" customWidth="1"/>
-    <col min="8" max="8" width="26.1640625" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" customWidth="1"/>
+    <col min="6" max="7" width="21.33203125" customWidth="1"/>
+    <col min="8" max="8" width="41.83203125" customWidth="1"/>
+    <col min="9" max="9" width="26.1640625" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="31" customFormat="1" ht="17.5" customHeight="1">
+    <row r="1" spans="1:18" s="31" customFormat="1" ht="17.5" customHeight="1">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -5102,49 +5112,52 @@
         <v>3</v>
       </c>
       <c r="G1" s="31" t="s">
+        <v>1305</v>
+      </c>
+      <c r="H1" s="31" t="s">
         <v>1272</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>1273</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="J1" s="31" t="s">
         <v>1276</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="K1" s="31" t="s">
         <v>1277</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="L1" s="31" t="s">
         <v>1278</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="M1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="N1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="O1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="P1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="Q1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="R1" s="31" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.5" customHeight="1">
+    <row r="2" spans="1:18" ht="17.5" customHeight="1">
       <c r="A2" s="15"/>
       <c r="B2" s="35"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:17" ht="17.5" customHeight="1">
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="1:18" ht="17.5" customHeight="1">
       <c r="A3" s="15"/>
       <c r="B3" s="40" t="s">
         <v>1310</v>
@@ -5157,8 +5170,9 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:17" ht="17.5" customHeight="1">
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:18" ht="17.5" customHeight="1">
       <c r="A4" s="15"/>
       <c r="B4" s="40" t="s">
         <v>1311</v>
@@ -5171,8 +5185,9 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:17" ht="17.5" customHeight="1">
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:18" ht="17.5" customHeight="1">
       <c r="A5" s="15"/>
       <c r="B5" s="35"/>
       <c r="C5" s="4"/>
@@ -5185,20 +5200,23 @@
       <c r="F5" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="37" t="s">
+        <v>1331</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>87</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>88</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="17.5" customHeight="1">
+    <row r="6" spans="1:18" ht="17.5" customHeight="1">
       <c r="A6" s="15"/>
       <c r="B6" s="35" t="s">
         <v>1262</v>
@@ -5213,9 +5231,10 @@
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="O6" s="12"/>
-    </row>
-    <row r="7" spans="1:17" ht="17.5" customHeight="1">
+      <c r="K6" s="4"/>
+      <c r="P6" s="12"/>
+    </row>
+    <row r="7" spans="1:18" ht="17.5" customHeight="1">
       <c r="A7" s="15"/>
       <c r="B7" s="40" t="s">
         <v>1312</v>
@@ -5228,9 +5247,10 @@
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
-      <c r="O7" s="12"/>
-    </row>
-    <row r="8" spans="1:17" ht="17.5" customHeight="1">
+      <c r="K7" s="4"/>
+      <c r="P7" s="12"/>
+    </row>
+    <row r="8" spans="1:18" ht="17.5" customHeight="1">
       <c r="A8" s="15"/>
       <c r="B8" s="35" t="s">
         <v>1264</v>
@@ -5243,9 +5263,10 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-      <c r="O8" s="12"/>
-    </row>
-    <row r="9" spans="1:17" ht="17.5" customHeight="1">
+      <c r="K8" s="4"/>
+      <c r="P8" s="12"/>
+    </row>
+    <row r="9" spans="1:18" ht="17.5" customHeight="1">
       <c r="A9" s="15"/>
       <c r="B9" s="35"/>
       <c r="C9" s="4"/>
@@ -5256,9 +5277,10 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
-      <c r="O9" s="12"/>
-    </row>
-    <row r="10" spans="1:17" ht="17.5" customHeight="1">
+      <c r="K9" s="4"/>
+      <c r="P9" s="12"/>
+    </row>
+    <row r="10" spans="1:18" ht="17.5" customHeight="1">
       <c r="A10" s="15"/>
       <c r="B10" s="35" t="s">
         <v>1262</v>
@@ -5273,9 +5295,10 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
-      <c r="O10" s="12"/>
-    </row>
-    <row r="11" spans="1:17" ht="17.5" customHeight="1">
+      <c r="K10" s="4"/>
+      <c r="P10" s="12"/>
+    </row>
+    <row r="11" spans="1:18" ht="17.5" customHeight="1">
       <c r="A11" s="15"/>
       <c r="B11" s="40" t="s">
         <v>1313</v>
@@ -5288,13 +5311,14 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-      <c r="M11" s="12"/>
+      <c r="K11" s="4"/>
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
-    </row>
-    <row r="12" spans="1:17" ht="17.5" customHeight="1">
+      <c r="R11" s="12"/>
+    </row>
+    <row r="12" spans="1:18" ht="17.5" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="35" t="s">
         <v>1264</v>
@@ -5307,13 +5331,14 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
-      <c r="M12" s="12"/>
+      <c r="K12" s="4"/>
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="12"/>
-    </row>
-    <row r="13" spans="1:17" ht="17.5" customHeight="1">
+      <c r="R12" s="12"/>
+    </row>
+    <row r="13" spans="1:18" ht="17.5" customHeight="1">
       <c r="A13" s="15"/>
       <c r="B13" s="35"/>
       <c r="C13" s="4"/>
@@ -5324,8 +5349,9 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:17" ht="17.5" customHeight="1">
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:18" ht="17.5" customHeight="1">
       <c r="A14" s="15"/>
       <c r="B14" s="40" t="s">
         <v>1314</v>
@@ -5338,8 +5364,9 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:17" ht="17.5" customHeight="1">
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:18" ht="17.5" customHeight="1">
       <c r="A15" s="15"/>
       <c r="B15" s="35"/>
       <c r="D15" s="41" t="s">
@@ -5351,17 +5378,17 @@
       <c r="F15" t="s">
         <v>224</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>225</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>164</v>
       </c>
-      <c r="L15" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="17.5" customHeight="1">
+      <c r="M15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="17.5" customHeight="1">
       <c r="A16" s="15"/>
       <c r="B16" s="35"/>
       <c r="D16" s="42" t="s">
@@ -5373,16 +5400,17 @@
       <c r="F16" s="18" t="s">
         <v>226</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="18"/>
+      <c r="H16" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="I16" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="J16" s="18"/>
-      <c r="L16" s="18"/>
-    </row>
-    <row r="17" spans="1:12" ht="17.5" customHeight="1">
+      <c r="K16" s="18"/>
+      <c r="M16" s="18"/>
+    </row>
+    <row r="17" spans="1:13" ht="17.5" customHeight="1">
       <c r="A17" s="15"/>
       <c r="B17" s="35"/>
       <c r="C17" s="18"/>
@@ -5393,9 +5421,10 @@
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
       <c r="J17" s="18"/>
-      <c r="L17" s="18"/>
-    </row>
-    <row r="18" spans="1:12" ht="17.5" customHeight="1">
+      <c r="K17" s="18"/>
+      <c r="M17" s="18"/>
+    </row>
+    <row r="18" spans="1:13" ht="17.5" customHeight="1">
       <c r="A18" s="15"/>
       <c r="B18" s="35"/>
       <c r="D18" s="42" t="s">
@@ -5407,15 +5436,16 @@
       <c r="F18" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="18"/>
+      <c r="H18" s="18" t="s">
         <v>230</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="I18" s="18" t="s">
         <v>231</v>
       </c>
-      <c r="L18" s="18"/>
-    </row>
-    <row r="19" spans="1:12" ht="17.5" customHeight="1">
+      <c r="M18" s="18"/>
+    </row>
+    <row r="19" spans="1:13" ht="17.5" customHeight="1">
       <c r="A19" s="15"/>
       <c r="B19" s="40" t="s">
         <v>1262</v>
@@ -5429,9 +5459,10 @@
       <c r="G19" s="18"/>
       <c r="H19" s="18"/>
       <c r="I19" s="18"/>
-      <c r="L19" s="18"/>
-    </row>
-    <row r="20" spans="1:12" ht="17.5" customHeight="1">
+      <c r="J19" s="18"/>
+      <c r="M19" s="18"/>
+    </row>
+    <row r="20" spans="1:13" ht="17.5" customHeight="1">
       <c r="A20" s="15"/>
       <c r="B20" s="35"/>
       <c r="D20" s="18"/>
@@ -5440,9 +5471,10 @@
       <c r="G20" s="18"/>
       <c r="H20" s="18"/>
       <c r="I20" s="18"/>
-      <c r="L20" s="18"/>
-    </row>
-    <row r="21" spans="1:12" ht="17.5" customHeight="1">
+      <c r="J20" s="18"/>
+      <c r="M20" s="18"/>
+    </row>
+    <row r="21" spans="1:13" ht="17.5" customHeight="1">
       <c r="A21" s="15"/>
       <c r="B21" s="35"/>
       <c r="D21" s="18" t="s">
@@ -5452,15 +5484,16 @@
       <c r="F21" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="G21" s="18"/>
+      <c r="H21" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="H21" s="18" t="s">
+      <c r="I21" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="L21" s="18"/>
-    </row>
-    <row r="22" spans="1:12" ht="17.5" customHeight="1">
+      <c r="M21" s="18"/>
+    </row>
+    <row r="22" spans="1:13" ht="17.5" customHeight="1">
       <c r="A22" s="15"/>
       <c r="B22" s="40" t="s">
         <v>1264</v>
@@ -5473,8 +5506,9 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="15"/>
       <c r="B23" s="35"/>
       <c r="C23" s="4"/>
@@ -5485,32 +5519,33 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="15"/>
       <c r="B24" s="35"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:13">
       <c r="A25" s="15"/>
       <c r="B25" s="35"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:13">
       <c r="A26" s="15"/>
       <c r="B26" s="35"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:13">
       <c r="A27" s="15"/>
       <c r="B27" s="35"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:13">
       <c r="A28" s="15"/>
       <c r="B28" s="35"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:13">
       <c r="A29" s="15"/>
       <c r="B29" s="35"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:13">
       <c r="A30" s="15"/>
       <c r="B30" s="35"/>
     </row>
@@ -5529,8 +5564,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AC826"/>
   <sheetViews>
-    <sheetView topLeftCell="A605" workbookViewId="0">
-      <selection activeCell="T671" sqref="T671"/>
+    <sheetView topLeftCell="A408" workbookViewId="0">
+      <selection activeCell="E422" sqref="E422"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -18337,7 +18372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -18485,10 +18520,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -18497,14 +18532,14 @@
     <col min="2" max="2" width="24.83203125" style="35" customWidth="1"/>
     <col min="3" max="3" width="31.83203125" customWidth="1"/>
     <col min="4" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="17.1640625" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" customWidth="1"/>
-    <col min="16" max="16" width="13.83203125" customWidth="1"/>
-    <col min="18" max="18" width="14.83203125" customWidth="1"/>
+    <col min="6" max="7" width="17.1640625" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" customWidth="1"/>
+    <col min="17" max="17" width="13.83203125" customWidth="1"/>
+    <col min="19" max="19" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="31" customFormat="1" ht="17.5" customHeight="1">
+    <row r="1" spans="1:19" s="31" customFormat="1" ht="17.5" customHeight="1">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -18524,43 +18559,46 @@
         <v>3</v>
       </c>
       <c r="G1" s="31" t="s">
+        <v>1305</v>
+      </c>
+      <c r="H1" s="31" t="s">
         <v>1272</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>1273</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="J1" s="31" t="s">
         <v>1276</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="K1" s="31" t="s">
         <v>1277</v>
       </c>
-      <c r="K1" s="31" t="s">
+      <c r="L1" s="31" t="s">
         <v>1278</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="M1" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="31" t="s">
+      <c r="N1" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="31" t="s">
+      <c r="O1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="P1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="32" t="s">
+      <c r="Q1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="R1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="S1" s="31" t="s">
         <v>1329</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.5" customHeight="1">
+    <row r="2" spans="1:19" ht="17.5" customHeight="1">
       <c r="A2" s="15"/>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -18569,26 +18607,26 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="L2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" s="33" customFormat="1" ht="17.5" customHeight="1">
+      <c r="K2" s="4"/>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="33" customFormat="1" ht="17.5" customHeight="1">
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
-      <c r="H3" s="34"/>
       <c r="I3" s="34"/>
       <c r="J3" s="34"/>
-    </row>
-    <row r="4" spans="1:18" ht="17.5" customHeight="1">
+      <c r="K3" s="34"/>
+    </row>
+    <row r="4" spans="1:19" ht="17.5" customHeight="1">
       <c r="A4" s="15" t="s">
         <v>1232</v>
       </c>
@@ -18597,11 +18635,11 @@
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-    </row>
-    <row r="5" spans="1:18" ht="17.5" customHeight="1">
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:19" ht="17.5" customHeight="1">
       <c r="A5" s="15"/>
       <c r="D5" s="42" t="s">
         <v>1318</v>
@@ -18612,19 +18650,19 @@
       <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="L5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="17.5" customHeight="1">
+      <c r="K5" s="4"/>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="17.5" customHeight="1">
       <c r="A6" s="15"/>
       <c r="B6" s="35" t="s">
         <v>1262</v>
@@ -18634,11 +18672,11 @@
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
-      <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="1:18" ht="17.5" customHeight="1">
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:19" ht="17.5" customHeight="1">
       <c r="A7" s="15"/>
       <c r="D7" s="4" t="s">
         <v>18</v>
@@ -18647,32 +18685,33 @@
       <c r="F7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="4"/>
+      <c r="H7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="I7" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="J7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L7" t="b">
-        <v>1</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
         <v>25</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>26</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="P7" s="12" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="17.5" customHeight="1">
+    <row r="8" spans="1:19" ht="17.5" customHeight="1">
       <c r="A8" s="15"/>
       <c r="B8" s="35" t="s">
         <v>1263</v>
@@ -18681,12 +18720,13 @@
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="18"/>
       <c r="J8" s="4"/>
-      <c r="O8" s="12"/>
-    </row>
-    <row r="9" spans="1:18" ht="17.5" customHeight="1">
+      <c r="K8" s="4"/>
+      <c r="P8" s="12"/>
+    </row>
+    <row r="9" spans="1:19" ht="17.5" customHeight="1">
       <c r="A9" s="15"/>
       <c r="D9" s="4" t="s">
         <v>28</v>
@@ -18695,24 +18735,25 @@
       <c r="F9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="4"/>
+      <c r="H9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="I9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="J9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="K9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L9" t="b">
-        <v>1</v>
-      </c>
-      <c r="O9" s="12"/>
-    </row>
-    <row r="10" spans="1:18" ht="17.5" customHeight="1">
+      <c r="M9" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" s="12"/>
+    </row>
+    <row r="10" spans="1:19" ht="17.5" customHeight="1">
       <c r="A10" s="15"/>
       <c r="B10" s="35" t="s">
         <v>1264</v>
@@ -18721,12 +18762,13 @@
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="18"/>
       <c r="J10" s="4"/>
-      <c r="O10" s="12"/>
-    </row>
-    <row r="11" spans="1:18" ht="17.5" customHeight="1">
+      <c r="K10" s="4"/>
+      <c r="P10" s="12"/>
+    </row>
+    <row r="11" spans="1:19" ht="17.5" customHeight="1">
       <c r="A11" s="15"/>
       <c r="B11" s="35" t="s">
         <v>34</v>
@@ -18736,22 +18778,24 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="18"/>
       <c r="J11" s="4"/>
-      <c r="O11" s="12"/>
-    </row>
-    <row r="12" spans="1:18" s="33" customFormat="1" ht="17.5" customHeight="1">
+      <c r="K11" s="4"/>
+      <c r="P11" s="12"/>
+    </row>
+    <row r="12" spans="1:19" s="33" customFormat="1" ht="17.5" customHeight="1">
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
       <c r="G12" s="34"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="34"/>
-    </row>
-    <row r="13" spans="1:18" ht="17.5" customHeight="1">
+      <c r="K12" s="34"/>
+    </row>
+    <row r="13" spans="1:19" ht="17.5" customHeight="1">
       <c r="A13" s="15" t="s">
         <v>1233</v>
       </c>
@@ -18768,8 +18812,9 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:18" ht="17.5" customHeight="1">
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:19" ht="17.5" customHeight="1">
       <c r="A14" s="15"/>
       <c r="D14" s="18" t="s">
         <v>42</v>
@@ -18778,30 +18823,33 @@
       <c r="F14" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="55" t="s">
+        <v>1332</v>
+      </c>
+      <c r="H14" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="I14" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="K14" s="18"/>
-      <c r="L14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="17.5" customHeight="1">
+      <c r="L14" s="18"/>
+      <c r="M14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="17.5" customHeight="1">
       <c r="A15" s="15"/>
       <c r="B15" s="35" t="s">
         <v>1265</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="17.5" customHeight="1">
+    <row r="16" spans="1:19" ht="17.5" customHeight="1">
       <c r="A16" s="15"/>
       <c r="B16" s="35" t="s">
         <v>1264</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="17.5" customHeight="1">
+    <row r="17" spans="1:18" ht="17.5" customHeight="1">
       <c r="A17" s="15"/>
       <c r="C17" s="18"/>
       <c r="D17" s="18" t="s">
@@ -18811,21 +18859,22 @@
       <c r="F17" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="18"/>
+      <c r="H17" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="I17" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="I17" s="18"/>
       <c r="J17" s="18"/>
-      <c r="M17" s="12"/>
+      <c r="K17" s="18"/>
       <c r="N17" s="12"/>
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
       <c r="Q17" s="12"/>
-    </row>
-    <row r="18" spans="1:17" ht="17.5" customHeight="1">
+      <c r="R17" s="12"/>
+    </row>
+    <row r="18" spans="1:18" ht="17.5" customHeight="1">
       <c r="A18" s="15"/>
       <c r="C18" s="18"/>
       <c r="D18" s="42" t="s">
@@ -18837,61 +18886,63 @@
       <c r="F18" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="18"/>
+      <c r="H18" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="I18" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="I18" s="18"/>
       <c r="J18" s="18"/>
-      <c r="M18" s="12"/>
+      <c r="K18" s="18"/>
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
       <c r="Q18" s="12"/>
-    </row>
-    <row r="19" spans="1:17" ht="17.5" customHeight="1">
+      <c r="R18" s="12"/>
+    </row>
+    <row r="19" spans="1:18" ht="17.5" customHeight="1">
       <c r="A19" s="15"/>
     </row>
-    <row r="20" spans="1:17" ht="17.5" customHeight="1">
+    <row r="20" spans="1:18" ht="17.5" customHeight="1">
       <c r="A20" s="15"/>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:18">
       <c r="A21" s="15"/>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:18">
       <c r="A22" s="15"/>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:18">
       <c r="A23" s="15"/>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:18">
       <c r="A24" s="15"/>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:18">
       <c r="A25" s="15"/>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:18">
       <c r="A26" s="15"/>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:18">
       <c r="A27" s="15"/>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:18">
       <c r="A28" s="15"/>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:18">
       <c r="A29" s="15"/>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:18">
       <c r="A30" s="15"/>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:18">
       <c r="A31" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -18904,8 +18955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -19371,8 +19422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -19637,8 +19688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R42"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -20034,7 +20085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R78" sqref="R78"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Made all the header navigation buttons fit on one line, added functionality to hide the navigation button text, fixed imnci form to finalize
</commit_message>
<xml_diff>
--- a/form-files/tables/imnci/forms/imnci_test/imnci_test.xlsx
+++ b/form-files/tables/imnci/forms/imnci_test/imnci_test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="460" windowWidth="25820" windowHeight="16220" firstSheet="4" activeTab="10"/>
+    <workbookView xWindow="3180" yWindow="0" windowWidth="45300" windowHeight="28220" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="10" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="1337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2835" uniqueCount="1339">
   <si>
     <t>comments</t>
   </si>
@@ -4251,6 +4251,12 @@
       </rPr>
       <t>if</t>
     </r>
+  </si>
+  <si>
+    <t>not(selected(data('birthdayKnown'), 'yes'))</t>
+  </si>
+  <si>
+    <t>hideNavigationButtonText</t>
   </si>
 </sst>
 </file>
@@ -4612,10 +4618,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="34" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4808,14 +4842,42 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -5118,8 +5180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R1048576"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -5603,8 +5665,8 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AB826"/>
   <sheetViews>
-    <sheetView topLeftCell="I174" workbookViewId="0">
-      <selection activeCell="R194" sqref="R194"/>
+    <sheetView topLeftCell="D627" workbookViewId="0">
+      <selection activeCell="N377" sqref="N377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -6151,14 +6213,14 @@
         <v>367</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="12">
+    <row r="39" spans="1:27" ht="24">
       <c r="A39" s="15"/>
       <c r="B39" s="53"/>
       <c r="C39" t="s">
         <v>14</v>
       </c>
-      <c r="N39" t="b">
-        <v>1</v>
+      <c r="N39" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="40" spans="1:27" ht="24">
@@ -6419,8 +6481,8 @@
       <c r="I59" t="s">
         <v>391</v>
       </c>
-      <c r="N59" t="b">
-        <v>1</v>
+      <c r="N59" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="60" spans="1:27" ht="24">
@@ -14785,8 +14847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="N148" sqref="N148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -14966,8 +15028,8 @@
       <c r="I9" t="s">
         <v>762</v>
       </c>
-      <c r="N9" t="b">
-        <v>1</v>
+      <c r="N9" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="16.75" customHeight="1">
@@ -14994,8 +15056,8 @@
       <c r="I11" t="s">
         <v>764</v>
       </c>
-      <c r="N11" t="b">
-        <v>1</v>
+      <c r="N11" t="s">
+        <v>1330</v>
       </c>
     </row>
     <row r="12" spans="1:27" ht="16.75" customHeight="1">
@@ -15033,8 +15095,8 @@
       <c r="J14" t="s">
         <v>767</v>
       </c>
-      <c r="N14" t="b">
-        <v>1</v>
+      <c r="N14" t="s">
+        <v>765</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="16.75" customHeight="1">
@@ -15216,8 +15278,8 @@
       <c r="J26" t="s">
         <v>767</v>
       </c>
-      <c r="N26" t="b">
-        <v>1</v>
+      <c r="N26" t="s">
+        <v>771</v>
       </c>
     </row>
     <row r="27" spans="1:27" ht="16.75" customHeight="1">
@@ -16545,6 +16607,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -17296,7 +17359,7 @@
   <dimension ref="A1:E98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
@@ -18357,10 +18420,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -18503,6 +18566,14 @@
         <v>1321</v>
       </c>
     </row>
+    <row r="14" spans="1:6" ht="12.75" customHeight="1">
+      <c r="A14" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B14" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -18518,8 +18589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -18692,8 +18763,8 @@
       <c r="K7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="M7" t="b">
-        <v>1</v>
+      <c r="M7" t="s">
+        <v>19</v>
       </c>
       <c r="N7" t="s">
         <v>1331</v>
@@ -18742,8 +18813,8 @@
       <c r="K9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="M9" t="b">
-        <v>1</v>
+      <c r="M9" t="s">
+        <v>1337</v>
       </c>
       <c r="P9" s="12"/>
     </row>
@@ -18827,8 +18898,8 @@
         <v>44</v>
       </c>
       <c r="L14" s="18"/>
-      <c r="M14" t="b">
-        <v>1</v>
+      <c r="M14" s="37" t="s">
+        <v>835</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="17.5" customHeight="1">
@@ -18947,8 +19018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -19411,8 +19482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -19557,8 +19628,8 @@
       </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="L6" t="b">
-        <v>1</v>
+      <c r="L6" s="4" t="s">
+        <v>1231</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="16.75" customHeight="1">
@@ -19661,6 +19732,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -19673,8 +19745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -20066,8 +20138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="L78" sqref="L78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -20188,8 +20260,8 @@
       <c r="H6" t="s">
         <v>143</v>
       </c>
-      <c r="L6" t="b">
-        <v>1</v>
+      <c r="L6" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="16.75" customHeight="1">
@@ -20328,8 +20400,8 @@
       <c r="H22" t="s">
         <v>155</v>
       </c>
-      <c r="L22" t="b">
-        <v>1</v>
+      <c r="L22" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:17" ht="16.75" customHeight="1">
@@ -20468,8 +20540,8 @@
       <c r="H35" t="s">
         <v>170</v>
       </c>
-      <c r="L35" t="b">
-        <v>1</v>
+      <c r="L35" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="16.75" customHeight="1">
@@ -20694,8 +20766,8 @@
       <c r="H53" t="s">
         <v>194</v>
       </c>
-      <c r="L53" t="b">
-        <v>1</v>
+      <c r="L53" s="12" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="54" spans="1:12" ht="16.75" customHeight="1">
@@ -20732,8 +20804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q59"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -20874,8 +20946,8 @@
       <c r="H7" t="s">
         <v>205</v>
       </c>
-      <c r="L7" t="b">
-        <v>1</v>
+      <c r="L7" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="17.5" customHeight="1">
@@ -21095,7 +21167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>
@@ -21417,8 +21489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC203"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView topLeftCell="A164" workbookViewId="0">
+      <selection activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>

</xml_diff>